<commit_message>
reword weekly schedule export
</commit_message>
<xml_diff>
--- a/Services/Report/Template/WeeklySchedule.xlsx
+++ b/Services/Report/Template/WeeklySchedule.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Thứ 2</t>
   </si>
@@ -45,49 +45,13 @@
   </si>
   <si>
     <t>Chủ Nhật</t>
-  </si>
-  <si>
-    <t>8:00 - 9:00</t>
-  </si>
-  <si>
-    <t>9:00 - 10:00</t>
-  </si>
-  <si>
-    <t>10:00 - 11:00</t>
-  </si>
-  <si>
-    <t>11:00 - 12:00</t>
-  </si>
-  <si>
-    <t>12:00 - 13:00</t>
-  </si>
-  <si>
-    <t>17:00 - 18:00</t>
-  </si>
-  <si>
-    <t>18:30 - 19:30</t>
-  </si>
-  <si>
-    <t>18:00 - 19:00</t>
-  </si>
-  <si>
-    <t>19:35 - 20:35</t>
-  </si>
-  <si>
-    <t>19:00 - 20:00</t>
-  </si>
-  <si>
-    <t>20:00 - 21:00</t>
-  </si>
-  <si>
-    <t>18:15 - 19:15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,40 +80,7 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="18"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color rgb="FFFF0000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="0" tint="-4.9989318521683403E-2"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color rgb="FFC00000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -239,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -262,38 +193,8 @@
     <xf numFmtId="14" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -575,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,184 +529,14 @@
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="6"/>
       <c r="E3" s="7"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" spans="1:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-    </row>
-    <row r="5" spans="1:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-    </row>
-    <row r="6" spans="1:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-    </row>
-    <row r="7" spans="1:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-    </row>
-    <row r="8" spans="1:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-    </row>
-    <row r="9" spans="1:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-    </row>
-    <row r="10" spans="1:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="12"/>
-    </row>
-    <row r="11" spans="1:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="12"/>
-    </row>
-    <row r="12" spans="1:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="12"/>
-    </row>
-    <row r="13" spans="1:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="12"/>
-    </row>
-    <row r="14" spans="1:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-    </row>
-    <row r="15" spans="1:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-    </row>
-    <row r="16" spans="1:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="1:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="6"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>